<commit_message>
Username and avatarid in get question
</commit_message>
<xml_diff>
--- a/Infofiles/Project_Apis_Quora.xlsx
+++ b/Infofiles/Project_Apis_Quora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\UK\QuoraStudent\Infofiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17079581-3A89-4507-B496-CD809899A59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0FDD4F-CACE-4D3C-81E4-396BBED2C428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,7 +378,9 @@
         "totalNumberOfComments": 1,
         "likedByTheRequestedUser": false,
         "disLikedByTheRequestedUser": true,
-        "questionOwnedByTheRequestedUser": true
+        "questionOwnedByTheRequestedUser": true,
+        "usernameOfWhoAskedThisQuestion": "vamsiirr",
+        "avataridOfWhoAskedThisQuestion": 1
     },
     "success": true,
     "reason": null
@@ -972,7 +974,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
get answers list and comments list on question or entity page request
</commit_message>
<xml_diff>
--- a/Infofiles/Project_Apis_Quora.xlsx
+++ b/Infofiles/Project_Apis_Quora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\UK\QuoraStudent\Infofiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0FDD4F-CACE-4D3C-81E4-396BBED2C428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614C3B8C-AAD8-469D-9E8F-51DFF55B7D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apis" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
   <si>
     <t xml:space="preserve">params </t>
   </si>
@@ -382,6 +382,119 @@
         "usernameOfWhoAskedThisQuestion": "vamsiirr",
         "avataridOfWhoAskedThisQuestion": 1
     },
+    "success": true,
+    "reason": null
+}</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/quoraStudent/answer/getAnswersForQuestionOrEntity</t>
+  </si>
+  <si>
+    <t>{
+    "eqid":2,
+    "ctype":"Q",
+    "userid":6
+}</t>
+  </si>
+  <si>
+    <t>{
+    "data": [
+        {
+            "aid": 1,
+            "eqid": 2,
+            "doa": 1658926096000,
+            "userid": 6,
+            "ctype": "Q",
+            "updatedat": 1658926096000,
+            "active": 1,
+            "content": "dont know :) ",
+            "answeredByUsername": "vamsi",
+            "answeredByUsernameAvatarid": "1",
+            "totalNumberOfLikes": 0,
+            "totalNumberOfDislikes": 0,
+            "totalNumberOfComments": 0,
+            "likedByTheRequestedUser": false,
+            "disLikedByTheRequestedUser": false,
+            "answerOwnedByTheRequestedUser": false
+        },
+        {
+            "aid": 2,
+            "eqid": 2,
+            "doa": 1658926130000,
+            "userid": 11,
+            "ctype": "Q",
+            "updatedat": 1658926130000,
+            "active": 1,
+            "content": "dont know :) how ",
+            "answeredByUsername": "vamsiirr",
+            "answeredByUsernameAvatarid": "1",
+            "totalNumberOfLikes": 1,
+            "totalNumberOfDislikes": 0,
+            "totalNumberOfComments": 0,
+            "likedByTheRequestedUser": false,
+            "disLikedByTheRequestedUser": false,
+            "answerOwnedByTheRequestedUser": false
+        }
+    ],
+    "success": true,
+    "reason": null
+}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/quoraStudent/comments/getCommentsList</t>
+  </si>
+  <si>
+    <t>{
+    "requestingUserId":6,
+    "ctype":"Q",
+    "eqabcid":2
+}</t>
+  </si>
+  <si>
+    <t>{
+    "data": [
+        {
+            "cid": 3,
+            "cpid": -1,
+            "userid": 6,
+            "parentid": 2,
+            "ctype": "Q",
+            "comment": "through portal !!! ",
+            "doc": 1657873175000,
+            "updatedat": 1657873175000,
+            "active": 1,
+            "commentedByUsername": "vamsi",
+            "commentedByUsernameAvatarid": 1,
+            "totalNumberOfLikes": 1,
+            "totalNumberOfDislikes": 0,
+            "totalNumberOfComments": 1,
+            "likedByTheRequestedUser": true,
+            "disLikedByTheRequestedUser": false,
+            "commentOwnedByTheRequestedUser": true
+        },
+        {
+            "cid": 4,
+            "cpid": -1,
+            "userid": 11,
+            "parentid": 2,
+            "ctype": "Q",
+            "comment": "through portal !!! ",
+            "doc": 1657873175000,
+            "updatedat": 1657873175000,
+            "active": 1,
+            "commentedByUsername": "vamsiirr",
+            "commentedByUsernameAvatarid": 1,
+            "totalNumberOfLikes": 0,
+            "totalNumberOfDislikes": 0,
+            "totalNumberOfComments": 1,
+            "likedByTheRequestedUser": false,
+            "disLikedByTheRequestedUser": false,
+            "commentOwnedByTheRequestedUser": false
+        }
+    ],
     "success": true,
     "reason": null
 }</t>
@@ -509,7 +622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -540,6 +653,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -971,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H26"/>
+  <dimension ref="B1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,35 +1328,35 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="B20" s="18" t="s">
+    <row r="20" spans="2:8" ht="409.6" x14ac:dyDescent="0.4">
+      <c r="B20" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="B21" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="H20" s="17"/>
-    </row>
-    <row r="21" spans="2:8" ht="409.6" x14ac:dyDescent="0.4">
-      <c r="B21" s="16" t="s">
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="H21" s="17"/>
+    </row>
+    <row r="22" spans="2:8" ht="164.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="147" x14ac:dyDescent="0.4">
-      <c r="B22" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>71</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>6</v>
@@ -1251,38 +1365,74 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="1" customFormat="1" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="19" t="s">
+    <row r="24" spans="2:8" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="2:8" ht="129.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="16" t="s">
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="2:8" ht="129.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C25" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="D25" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="185.7" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:8" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="17"/>
+    </row>
+    <row r="28" spans="2:8" ht="147" x14ac:dyDescent="0.4">
+      <c r="B28" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="409.6" x14ac:dyDescent="0.4">
+      <c r="B29" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B15" r:id="rId1" xr:uid="{7692C306-4A78-4B2D-948D-3A51CCED86C1}"/>
     <hyperlink ref="B17" r:id="rId2" xr:uid="{937B7D2A-8852-4A7B-82AD-E8F17830A145}"/>
     <hyperlink ref="B18" r:id="rId3" xr:uid="{FF691430-CFF3-45C6-9847-B201285A1D75}"/>
     <hyperlink ref="B19" r:id="rId4" xr:uid="{C7C540F5-786B-4C6A-B845-D1AE5BE717D8}"/>
-    <hyperlink ref="B21" r:id="rId5" xr:uid="{11ACBF41-FA7A-455E-8522-698BD9AA4BB0}"/>
-    <hyperlink ref="B24" r:id="rId6" xr:uid="{D169E3B6-2393-46B8-8832-573FD077AEBC}"/>
+    <hyperlink ref="B22" r:id="rId5" xr:uid="{11ACBF41-FA7A-455E-8522-698BD9AA4BB0}"/>
+    <hyperlink ref="B25" r:id="rId6" xr:uid="{D169E3B6-2393-46B8-8832-573FD077AEBC}"/>
+    <hyperlink ref="B28" r:id="rId7" xr:uid="{4BA1F53D-94A7-4CF9-AE6A-D7769CF57EA8}"/>
+    <hyperlink ref="B29" r:id="rId8" xr:uid="{0EFEC909-D5F0-41FA-9A9B-EC666481CA2E}"/>
+    <hyperlink ref="B20" r:id="rId9" xr:uid="{F31C776E-2D88-4733-858D-B77E048242B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>